<commit_message>
Screen Design Standards added
</commit_message>
<xml_diff>
--- a/MS2/workinprogress/Arbeitsmappe1.xlsx
+++ b/MS2/workinprogress/Arbeitsmappe1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Menu Contents</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Jspinner</t>
+  </si>
+  <si>
+    <t>Textfelder, Buttons, Kamera</t>
+  </si>
+  <si>
+    <t>Input des Benutzers</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A14" sqref="A14:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,64 +514,72 @@
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>